<commit_message>
mapping.xlsx - added magic_item_table sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/init_db_design/mapping.xlsx
+++ b/src/main/resources/init_db_design/mapping.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="magic_item" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="rarity" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="category" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="magic_item_table" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
   <si>
     <t xml:space="preserve">property</t>
   </si>
@@ -289,6 +290,54 @@
   </si>
   <si>
     <t xml:space="preserve">wondrous item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u_uid_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_category_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_rarity_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b_attunement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d_last_update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t_write</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uuid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number .2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timestamp</t>
   </si>
 </sst>
 </file>
@@ -417,11 +466,11 @@
   </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="76.69"/>
@@ -569,7 +618,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -664,7 +713,7 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.79"/>
@@ -730,6 +779,103 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.75"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mapping.xlsx - added table schemas for t_magic_item and related enums
</commit_message>
<xml_diff>
--- a/src/main/resources/init_db_design/mapping.xlsx
+++ b/src/main/resources/init_db_design/mapping.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="magic_item" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="rarity" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="category" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="magic_item_table" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="t_magic_item" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="e_rarity" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="e_category" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
   <si>
     <t xml:space="preserve">property</t>
   </si>
@@ -316,7 +318,10 @@
     <t xml:space="preserve">b_attunement</t>
   </si>
   <si>
-    <t xml:space="preserve">d_last_update</t>
+    <t xml:space="preserve">d_from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d_to</t>
   </si>
   <si>
     <t xml:space="preserve">t_write</t>
@@ -338,6 +343,30 @@
   </si>
   <si>
     <t xml:space="preserve">timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FK e_category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FK e_rarity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_from_character_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_value_from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_value_to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b_valid</t>
   </si>
 </sst>
 </file>
@@ -470,7 +499,7 @@
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="76.69"/>
@@ -615,10 +644,10 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
@@ -713,7 +742,7 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.79"/>
@@ -797,13 +826,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.47"/>
@@ -845,37 +874,190 @@
       <c r="J1" s="0" t="s">
         <v>62</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>63</v>
       </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>64</v>
+      </c>
       <c r="B2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>64</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>66</v>
+      </c>
       <c r="C2" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>